<commit_message>
Add TODOs for exploring techs per site
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbecker\JuliaPlay\oshkosh-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF062A81-8A94-4F7E-912D-0DF3740D135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089A3B6B-A469-4273-8443-4CAE1AACAAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2145" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="199">
   <si>
     <t>City</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>Operating Shifts</t>
-  </si>
-  <si>
-    <t>2-3</t>
   </si>
   <si>
     <t>Jason Grentus</t>
@@ -660,6 +657,9 @@
   </si>
   <si>
     <t>Wind Size kW</t>
+  </si>
+  <si>
+    <t>storageplustech</t>
   </si>
 </sst>
 </file>
@@ -748,12 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -780,6 +774,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1084,122 +1084,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>154</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="9">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="D2" s="11">
-        <v>6</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="9">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="D3" s="11">
-        <v>12</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="9">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="D5" s="11">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="D7" s="11">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1212,10 +1212,10 @@
   <dimension ref="A1:AF38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1228,7 @@
     <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1271,8 +1271,8 @@
       <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>146</v>
+      <c r="I1" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>138</v>
@@ -1301,47 +1301,47 @@
       <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="T1" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="V1" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="W1" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD1" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="AA1" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AE1" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="12" t="s">
         <v>188</v>
-      </c>
-      <c r="AF1" s="14" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,12 +1364,12 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="4">
         <v>525000</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="7">
         <v>96.25</v>
       </c>
       <c r="J2" s="6">
@@ -1396,60 +1396,60 @@
       <c r="Q2" s="3">
         <v>971213.25353999995</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9">
+      <c r="R2" s="7"/>
+      <c r="S2" s="7">
         <f>K2/8760</f>
         <v>2079.0926361872148</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="7">
         <f>P2/8760</f>
         <v>15.053209195205479</v>
       </c>
-      <c r="U2" s="19">
+      <c r="U2" s="17">
         <f>T2/0.4*1000000/3412*0.35*0.8</f>
         <v>3088.2902803762699</v>
       </c>
-      <c r="V2" s="19">
+      <c r="V2" s="17">
         <f>S2/0.2</f>
         <v>10395.463180936073</v>
       </c>
-      <c r="W2" s="19">
+      <c r="W2" s="17">
         <f>S2/0.35</f>
         <v>5940.2646748206143</v>
       </c>
-      <c r="X2" s="15">
+      <c r="X2" s="13">
         <f>M2/K2</f>
         <v>7.8293532609545233E-2</v>
       </c>
-      <c r="Y2" s="16">
+      <c r="Y2" s="14">
         <f>Q2/P2</f>
         <v>7.365146623032075</v>
       </c>
-      <c r="Z2" s="17">
+      <c r="Z2" s="15">
         <f>K2/(P2*1000000/3412)</f>
         <v>0.47125260684812692</v>
       </c>
-      <c r="AA2" s="18">
+      <c r="AA2" s="16">
         <f>L2/(K2/8760)</f>
         <v>1.9371431219081756</v>
       </c>
-      <c r="AB2" s="18">
+      <c r="AB2" s="16">
         <f t="shared" ref="AB2:AB28" si="0">L2/(K2/8760/(2/3))</f>
         <v>1.2914287479387836</v>
       </c>
-      <c r="AC2" s="18">
+      <c r="AC2" s="16">
         <f>L2/(K2/8760/(2/3*5/7))</f>
         <v>0.92244910567055982</v>
       </c>
-      <c r="AD2" s="17">
+      <c r="AD2" s="15">
         <f>I2*43560/H2</f>
         <v>7.9859999999999998</v>
       </c>
-      <c r="AE2" s="12">
+      <c r="AE2" s="10">
         <f>I2*43560/(H2/2)</f>
         <v>15.972</v>
       </c>
-      <c r="AF2" s="18">
+      <c r="AF2" s="16">
         <f>(AE2-1)*I2</f>
         <v>1441.0550000000001</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" s="4">
         <v>479139</v>
@@ -1482,8 +1482,8 @@
       <c r="I3" s="1">
         <v>43.7</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>139</v>
+      <c r="J3" s="19">
+        <v>2</v>
       </c>
       <c r="K3" s="4">
         <v>11428742.6</v>
@@ -1507,61 +1507,61 @@
         <v>461473.59</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="S3" s="9">
+        <v>149</v>
+      </c>
+      <c r="S3" s="7">
         <f t="shared" ref="S3:S28" si="1">K3/8760</f>
         <v>1304.6509817351598</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="7">
         <f t="shared" ref="T3:T28" si="2">P3/8760</f>
         <v>10.824060502283105</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="17">
         <f t="shared" ref="U3:U28" si="3">T3/0.4*1000000/3412*0.35*0.8</f>
         <v>2220.6454723324073</v>
       </c>
-      <c r="V3" s="19">
+      <c r="V3" s="17">
         <f t="shared" ref="V3:V28" si="4">S3/0.2</f>
         <v>6523.254908675799</v>
       </c>
-      <c r="W3" s="19">
+      <c r="W3" s="17">
         <f t="shared" ref="W3:W28" si="5">S3/0.35</f>
         <v>3727.5742335290283</v>
       </c>
-      <c r="X3" s="15">
+      <c r="X3" s="13">
         <f t="shared" ref="X3:X28" si="6">M3/K3</f>
         <v>0.10801228474600523</v>
       </c>
-      <c r="Y3" s="16">
+      <c r="Y3" s="14">
         <f t="shared" ref="Y3:Y28" si="7">Q3/P3</f>
         <v>4.8669012475061635</v>
       </c>
-      <c r="Z3" s="17">
+      <c r="Z3" s="15">
         <f t="shared" ref="Z3:Z28" si="8">K3/(P3*1000000/3412)</f>
         <v>0.41125686139147338</v>
       </c>
-      <c r="AA3" s="18">
+      <c r="AA3" s="16">
         <f t="shared" ref="AA3:AA28" si="9">L3/(K3/8760)</f>
         <v>1.6510162719037875</v>
       </c>
-      <c r="AB3" s="18">
+      <c r="AB3" s="16">
         <f t="shared" si="0"/>
         <v>1.1006775146025249</v>
       </c>
-      <c r="AC3" s="18">
+      <c r="AC3" s="16">
         <f t="shared" ref="AC3:AC28" si="10">L3/(K3/8760/(2/3*5/7))</f>
         <v>0.78619822471608924</v>
       </c>
-      <c r="AD3" s="17">
+      <c r="AD3" s="15">
         <f t="shared" ref="AD3:AD28" si="11">I3*43560/H3</f>
         <v>3.9729013918716705</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="10">
         <f t="shared" ref="AE3:AE28" si="12">I3*43560/(H3/2)</f>
         <v>7.9458027837433409</v>
       </c>
-      <c r="AF3" s="18">
+      <c r="AF3" s="16">
         <f t="shared" ref="AF3:AF28" si="13">(AE3-1)*I3</f>
         <v>303.53158164958404</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" s="4">
         <v>385400</v>
@@ -1594,8 +1594,8 @@
       <c r="I4" s="1">
         <v>48.1</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>139</v>
+      <c r="J4" s="19">
+        <v>2</v>
       </c>
       <c r="K4" s="4">
         <v>6277299.6900000004</v>
@@ -1618,64 +1618,64 @@
       <c r="Q4" s="5">
         <v>169291.44</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="7">
         <f t="shared" si="1"/>
         <v>716.58672260273977</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="7">
         <f t="shared" si="2"/>
         <v>4.1384166666666662</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U4" s="17">
         <f t="shared" si="3"/>
         <v>849.03038296209434</v>
       </c>
-      <c r="V4" s="19">
+      <c r="V4" s="17">
         <f t="shared" si="4"/>
         <v>3582.9336130136985</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W4" s="17">
         <f t="shared" si="5"/>
         <v>2047.3906360078281</v>
       </c>
-      <c r="X4" s="15">
+      <c r="X4" s="13">
         <f t="shared" si="6"/>
         <v>0.11687476243467355</v>
       </c>
-      <c r="Y4" s="16">
+      <c r="Y4" s="14">
         <f t="shared" si="7"/>
         <v>4.6697827710231534</v>
       </c>
-      <c r="Z4" s="17">
+      <c r="Z4" s="15">
         <f t="shared" si="8"/>
         <v>0.59080418779820343</v>
       </c>
-      <c r="AA4" s="18">
+      <c r="AA4" s="16">
         <f t="shared" si="9"/>
         <v>3.2571075159229812</v>
       </c>
-      <c r="AB4" s="18">
+      <c r="AB4" s="16">
         <f t="shared" si="0"/>
         <v>2.1714050106153202</v>
       </c>
-      <c r="AC4" s="18">
+      <c r="AC4" s="16">
         <f t="shared" si="10"/>
         <v>1.5510035790109433</v>
       </c>
-      <c r="AD4" s="17">
+      <c r="AD4" s="15">
         <f t="shared" si="11"/>
         <v>5.4365230928905035</v>
       </c>
-      <c r="AE4" s="12">
+      <c r="AE4" s="10">
         <f t="shared" si="12"/>
         <v>10.873046185781007</v>
       </c>
-      <c r="AF4" s="18">
+      <c r="AF4" s="16">
         <f t="shared" si="13"/>
         <v>474.89352153606643</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5" s="4">
         <v>486656</v>
@@ -1703,8 +1703,8 @@
       <c r="I5" s="1">
         <v>63.3</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>139</v>
+      <c r="J5" s="19">
+        <v>2</v>
       </c>
       <c r="K5" s="4">
         <v>11848853.33333</v>
@@ -1728,59 +1728,59 @@
       <c r="R5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="7">
         <f t="shared" si="1"/>
         <v>1352.6088280057077</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="7">
         <f t="shared" si="2"/>
         <v>0.20205721575342467</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="17">
         <f t="shared" si="3"/>
         <v>41.453707804043745</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="17">
         <f t="shared" si="4"/>
         <v>6763.0441400285381</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="17">
         <f t="shared" si="5"/>
         <v>3864.5966514448792</v>
       </c>
-      <c r="X5" s="15">
+      <c r="X5" s="13">
         <f t="shared" si="6"/>
         <v>7.108103340944133E-2</v>
       </c>
-      <c r="Y5" s="16">
+      <c r="Y5" s="14">
         <f t="shared" si="7"/>
         <v>16.98770398350198</v>
       </c>
-      <c r="Z5" s="17">
+      <c r="Z5" s="15">
         <f t="shared" si="8"/>
         <v>22.840566737232464</v>
       </c>
-      <c r="AA5" s="18">
+      <c r="AA5" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AB5" s="18">
+      <c r="AB5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="18">
+      <c r="AC5" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="17">
+      <c r="AD5" s="15">
         <f t="shared" si="11"/>
         <v>5.6659077459231986</v>
       </c>
-      <c r="AE5" s="12">
+      <c r="AE5" s="10">
         <f t="shared" si="12"/>
         <v>11.331815491846397</v>
       </c>
-      <c r="AF5" s="18">
+      <c r="AF5" s="16">
         <f t="shared" si="13"/>
         <v>654.00392063387687</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H6" s="4">
         <v>710899</v>
@@ -1813,8 +1813,8 @@
       <c r="I6" s="1">
         <v>151.1</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>139</v>
+      <c r="J6" s="19">
+        <v>2</v>
       </c>
       <c r="K6" s="4">
         <v>11553668.29934</v>
@@ -1837,59 +1837,59 @@
       <c r="Q6" s="3">
         <v>1073601.65808</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="7">
         <f t="shared" si="1"/>
         <v>1318.9119063173516</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="7">
         <f t="shared" si="2"/>
         <v>14.743516389269406</v>
       </c>
-      <c r="U6" s="19">
+      <c r="U6" s="17">
         <f t="shared" si="3"/>
         <v>3024.7542416437818</v>
       </c>
-      <c r="V6" s="19">
+      <c r="V6" s="17">
         <f t="shared" si="4"/>
         <v>6594.5595315867577</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="17">
         <f t="shared" si="5"/>
         <v>3768.3197323352906</v>
       </c>
-      <c r="X6" s="15">
+      <c r="X6" s="13">
         <f t="shared" si="6"/>
         <v>0.1307292003671493</v>
       </c>
-      <c r="Y6" s="16">
+      <c r="Y6" s="14">
         <f t="shared" si="7"/>
         <v>8.3126212002795317</v>
       </c>
-      <c r="Z6" s="17">
+      <c r="Z6" s="15">
         <f t="shared" si="8"/>
         <v>0.30522755260950341</v>
       </c>
-      <c r="AA6" s="18">
+      <c r="AA6" s="16">
         <f t="shared" si="9"/>
         <v>3.2038910102789226</v>
       </c>
-      <c r="AB6" s="18">
+      <c r="AB6" s="16">
         <f t="shared" si="0"/>
         <v>2.1359273401859484</v>
       </c>
-      <c r="AC6" s="18">
+      <c r="AC6" s="16">
         <f t="shared" si="10"/>
         <v>1.5256623858471061</v>
       </c>
-      <c r="AD6" s="17">
+      <c r="AD6" s="15">
         <f t="shared" si="11"/>
         <v>9.2585810361246814</v>
       </c>
-      <c r="AE6" s="12">
+      <c r="AE6" s="10">
         <f t="shared" si="12"/>
         <v>18.517162072249363</v>
       </c>
-      <c r="AF6" s="18">
+      <c r="AF6" s="16">
         <f t="shared" si="13"/>
         <v>2646.8431891168784</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="4">
         <v>486000</v>
@@ -1922,8 +1922,8 @@
       <c r="I7" s="1">
         <v>81.260000000000005</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>139</v>
+      <c r="J7" s="19">
+        <v>2</v>
       </c>
       <c r="K7" s="4">
         <v>11025473.666309999</v>
@@ -1947,61 +1947,61 @@
         <v>714293.53193000006</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="S7" s="9">
+        <v>147</v>
+      </c>
+      <c r="S7" s="7">
         <f t="shared" si="1"/>
         <v>1258.6157153321917</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="7">
         <f t="shared" si="2"/>
         <v>18.745163352739727</v>
       </c>
-      <c r="U7" s="19">
+      <c r="U7" s="17">
         <f t="shared" si="3"/>
         <v>3845.7251896007651</v>
       </c>
-      <c r="V7" s="19">
+      <c r="V7" s="17">
         <f t="shared" si="4"/>
         <v>6293.0785766609579</v>
       </c>
-      <c r="W7" s="19">
+      <c r="W7" s="17">
         <f t="shared" si="5"/>
         <v>3596.0449009491194</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="13">
         <f t="shared" si="6"/>
         <v>8.4001571950601359E-2</v>
       </c>
-      <c r="Y7" s="16">
+      <c r="Y7" s="14">
         <f t="shared" si="7"/>
         <v>4.3499411550520346</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="15">
         <f t="shared" si="8"/>
         <v>0.22909359283261643</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AA7" s="16">
         <f t="shared" si="9"/>
         <v>1.7002806924551874</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AB7" s="16">
         <f t="shared" si="0"/>
         <v>1.1335204616367915</v>
       </c>
-      <c r="AC7" s="18">
+      <c r="AC7" s="16">
         <f t="shared" si="10"/>
         <v>0.80965747259770826</v>
       </c>
-      <c r="AD7" s="17">
+      <c r="AD7" s="15">
         <f t="shared" si="11"/>
         <v>7.2833037037037043</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AE7" s="10">
         <f t="shared" si="12"/>
         <v>14.566607407407409</v>
       </c>
-      <c r="AF7" s="18">
+      <c r="AF7" s="16">
         <f t="shared" si="13"/>
         <v>1102.4225179259261</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="4">
         <v>930000</v>
@@ -2061,59 +2061,59 @@
       <c r="R8" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="7">
         <f t="shared" si="1"/>
         <v>761.67096595433782</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="7">
         <f t="shared" si="2"/>
         <v>1.5233578550228311</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="17">
         <f t="shared" si="3"/>
         <v>312.52945443024089</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="17">
         <f t="shared" si="4"/>
         <v>3808.3548297716889</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="17">
         <f t="shared" si="5"/>
         <v>2176.2027598695367</v>
       </c>
-      <c r="X8" s="15">
+      <c r="X8" s="13">
         <f t="shared" si="6"/>
         <v>0.11714809607723407</v>
       </c>
-      <c r="Y8" s="16">
+      <c r="Y8" s="14">
         <f t="shared" si="7"/>
         <v>9.2645707223676705</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="Z8" s="15">
         <f t="shared" si="8"/>
         <v>1.7059821677929059</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AA8" s="16">
         <f t="shared" si="9"/>
         <v>4.6681574576562737</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AB8" s="16">
         <f t="shared" si="0"/>
         <v>3.1121049717708491</v>
       </c>
-      <c r="AC8" s="18">
+      <c r="AC8" s="16">
         <f t="shared" si="10"/>
         <v>2.2229321226934635</v>
       </c>
-      <c r="AD8" s="17">
+      <c r="AD8" s="15">
         <f t="shared" si="11"/>
         <v>4.5386709677419352</v>
       </c>
-      <c r="AE8" s="12">
+      <c r="AE8" s="10">
         <f t="shared" si="12"/>
         <v>9.0773419354838705</v>
       </c>
-      <c r="AF8" s="18">
+      <c r="AF8" s="16">
         <f t="shared" si="13"/>
         <v>782.69443354838711</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="4">
         <v>249000</v>
@@ -2146,8 +2146,8 @@
       <c r="I9" s="1">
         <v>14.4</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>139</v>
+      <c r="J9" s="18">
+        <v>2</v>
       </c>
       <c r="K9" s="4">
         <v>4934116.9999900004</v>
@@ -2170,59 +2170,59 @@
       <c r="Q9" s="3">
         <v>101490.89859</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="7">
         <f t="shared" si="1"/>
         <v>563.25536529566216</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="7">
         <f t="shared" si="2"/>
         <v>1.948352390410959</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="17">
         <f t="shared" si="3"/>
         <v>399.72059592252964</v>
       </c>
-      <c r="V9" s="19">
+      <c r="V9" s="17">
         <f t="shared" si="4"/>
         <v>2816.2768264783108</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="17">
         <f t="shared" si="5"/>
         <v>1609.301043701892</v>
       </c>
-      <c r="X9" s="15">
+      <c r="X9" s="13">
         <f t="shared" si="6"/>
         <v>0.10588080890888052</v>
       </c>
-      <c r="Y9" s="16">
+      <c r="Y9" s="14">
         <f t="shared" si="7"/>
         <v>5.9464186633505003</v>
       </c>
-      <c r="Z9" s="17">
+      <c r="Z9" s="15">
         <f t="shared" si="8"/>
         <v>0.98638588986637843</v>
       </c>
-      <c r="AA9" s="18">
+      <c r="AA9" s="16">
         <f t="shared" si="9"/>
         <v>2.1943865538701135</v>
       </c>
-      <c r="AB9" s="18">
+      <c r="AB9" s="16">
         <f t="shared" si="0"/>
         <v>1.4629243692467424</v>
       </c>
-      <c r="AC9" s="18">
+      <c r="AC9" s="16">
         <f t="shared" si="10"/>
         <v>1.0449459780333874</v>
       </c>
-      <c r="AD9" s="17">
+      <c r="AD9" s="15">
         <f t="shared" si="11"/>
         <v>2.5191325301204821</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AE9" s="10">
         <f t="shared" si="12"/>
         <v>5.0382650602409642</v>
       </c>
-      <c r="AF9" s="18">
+      <c r="AF9" s="16">
         <f t="shared" si="13"/>
         <v>58.151016867469885</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H10" s="4">
         <v>300334</v>
@@ -2255,8 +2255,8 @@
       <c r="I10" s="1">
         <v>32.9</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>139</v>
+      <c r="J10" s="18">
+        <v>2</v>
       </c>
       <c r="K10" s="4">
         <v>4847935.5258499999</v>
@@ -2279,59 +2279,59 @@
       <c r="Q10" s="3">
         <v>60303.547180000001</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="7">
         <f t="shared" si="1"/>
         <v>553.41729747146121</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="7">
         <f t="shared" si="2"/>
         <v>0.97806170547945215</v>
       </c>
-      <c r="U10" s="19">
+      <c r="U10" s="17">
         <f t="shared" si="3"/>
         <v>200.65744250750777</v>
       </c>
-      <c r="V10" s="19">
+      <c r="V10" s="17">
         <f t="shared" si="4"/>
         <v>2767.0864873573059</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="17">
         <f t="shared" si="5"/>
         <v>1581.1922784898893</v>
       </c>
-      <c r="X10" s="15">
+      <c r="X10" s="13">
         <f t="shared" si="6"/>
         <v>0.10489337687527119</v>
       </c>
-      <c r="Y10" s="16">
+      <c r="Y10" s="14">
         <f t="shared" si="7"/>
         <v>7.038376550776821</v>
       </c>
-      <c r="Z10" s="17">
+      <c r="Z10" s="15">
         <f t="shared" si="8"/>
         <v>1.9306142019403452</v>
       </c>
-      <c r="AA10" s="18">
+      <c r="AA10" s="16">
         <f t="shared" si="9"/>
         <v>2.1791873971235809</v>
       </c>
-      <c r="AB10" s="18">
+      <c r="AB10" s="16">
         <f t="shared" si="0"/>
         <v>1.4527915980823871</v>
       </c>
-      <c r="AC10" s="18">
+      <c r="AC10" s="16">
         <f t="shared" si="10"/>
         <v>1.0377082843445622</v>
       </c>
-      <c r="AD10" s="17">
+      <c r="AD10" s="15">
         <f t="shared" si="11"/>
         <v>4.771767432258752</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AE10" s="10">
         <f t="shared" si="12"/>
         <v>9.543534864517504</v>
       </c>
-      <c r="AF10" s="18">
+      <c r="AF10" s="16">
         <f t="shared" si="13"/>
         <v>281.0822970426259</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="4">
         <v>302000</v>
@@ -2364,8 +2364,8 @@
       <c r="I11" s="1">
         <v>35.700000000000003</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>139</v>
+      <c r="J11" s="18">
+        <v>2</v>
       </c>
       <c r="K11" s="4">
         <v>3879818.3397900001</v>
@@ -2388,59 +2388,59 @@
       <c r="Q11" s="3">
         <v>139842.81967999999</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="7">
         <f t="shared" si="1"/>
         <v>442.90163696232878</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="7">
         <f t="shared" si="2"/>
         <v>3.2378365742009132</v>
       </c>
-      <c r="U11" s="19">
+      <c r="U11" s="17">
         <f t="shared" si="3"/>
         <v>664.26893374579095</v>
       </c>
-      <c r="V11" s="19">
+      <c r="V11" s="17">
         <f t="shared" si="4"/>
         <v>2214.5081848116438</v>
       </c>
-      <c r="W11" s="19">
+      <c r="W11" s="17">
         <f t="shared" si="5"/>
         <v>1265.4332484637966</v>
       </c>
-      <c r="X11" s="15">
+      <c r="X11" s="13">
         <f t="shared" si="6"/>
         <v>9.9339549469953103E-2</v>
       </c>
-      <c r="Y11" s="16">
+      <c r="Y11" s="14">
         <f t="shared" si="7"/>
         <v>4.930388497094869</v>
       </c>
-      <c r="Z11" s="17">
+      <c r="Z11" s="15">
         <f t="shared" si="8"/>
         <v>0.4667253428899264</v>
       </c>
-      <c r="AA11" s="18">
+      <c r="AA11" s="16">
         <f t="shared" si="9"/>
         <v>2.7748824963239711</v>
       </c>
-      <c r="AB11" s="18">
+      <c r="AB11" s="16">
         <f t="shared" si="0"/>
         <v>1.8499216642159804</v>
       </c>
-      <c r="AC11" s="18">
+      <c r="AC11" s="16">
         <f t="shared" si="10"/>
         <v>1.321372617297129</v>
       </c>
-      <c r="AD11" s="17">
+      <c r="AD11" s="15">
         <f t="shared" si="11"/>
         <v>5.1493112582781464</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AE11" s="10">
         <f t="shared" si="12"/>
         <v>10.298622516556293</v>
       </c>
-      <c r="AF11" s="18">
+      <c r="AF11" s="16">
         <f t="shared" si="13"/>
         <v>331.96082384105966</v>
       </c>
@@ -2465,12 +2465,12 @@
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H12" s="4">
         <v>320000</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <f>40.4+2.52</f>
         <v>42.92</v>
       </c>
@@ -2498,59 +2498,59 @@
       <c r="Q12" s="3">
         <v>103018.02</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="7">
         <f t="shared" si="1"/>
         <v>367.84281674429224</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="7">
         <f t="shared" si="2"/>
         <v>0.86665262557077627</v>
       </c>
-      <c r="U12" s="19">
+      <c r="U12" s="17">
         <f t="shared" si="3"/>
         <v>177.8009489740748</v>
       </c>
-      <c r="V12" s="19">
+      <c r="V12" s="17">
         <f t="shared" si="4"/>
         <v>1839.2140837214611</v>
       </c>
-      <c r="W12" s="19">
+      <c r="W12" s="17">
         <f t="shared" si="5"/>
         <v>1050.9794764122637</v>
       </c>
-      <c r="X12" s="15">
+      <c r="X12" s="13">
         <f t="shared" si="6"/>
         <v>8.5916331345552654E-2</v>
       </c>
-      <c r="Y12" s="16">
+      <c r="Y12" s="14">
         <f t="shared" si="7"/>
         <v>13.569505933776323</v>
       </c>
-      <c r="Z12" s="17">
+      <c r="Z12" s="15">
         <f t="shared" si="8"/>
         <v>1.4481923364680644</v>
       </c>
-      <c r="AA12" s="18">
+      <c r="AA12" s="16">
         <f t="shared" si="9"/>
         <v>1.4870482040165807</v>
       </c>
-      <c r="AB12" s="18">
+      <c r="AB12" s="16">
         <f t="shared" si="0"/>
         <v>0.99136546934438707</v>
       </c>
-      <c r="AC12" s="18">
+      <c r="AC12" s="16">
         <f t="shared" si="10"/>
         <v>0.70811819238884788</v>
       </c>
-      <c r="AD12" s="17">
+      <c r="AD12" s="15">
         <f t="shared" si="11"/>
         <v>5.8424850000000008</v>
       </c>
-      <c r="AE12" s="12">
+      <c r="AE12" s="10">
         <f t="shared" si="12"/>
         <v>11.684970000000002</v>
       </c>
-      <c r="AF12" s="18">
+      <c r="AF12" s="16">
         <f t="shared" si="13"/>
         <v>458.59891240000007</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H13" s="4">
         <v>262000</v>
@@ -2607,59 +2607,59 @@
       <c r="Q13" s="3">
         <v>262482.42</v>
       </c>
-      <c r="S13" s="9">
+      <c r="S13" s="7">
         <f t="shared" si="1"/>
         <v>361.97135807876714</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="7">
         <f t="shared" si="2"/>
         <v>3.654241874429224</v>
       </c>
-      <c r="U13" s="19">
+      <c r="U13" s="17">
         <f t="shared" si="3"/>
         <v>749.69792265546801</v>
       </c>
-      <c r="V13" s="19">
+      <c r="V13" s="17">
         <f t="shared" si="4"/>
         <v>1809.8567903938356</v>
       </c>
-      <c r="W13" s="19">
+      <c r="W13" s="17">
         <f t="shared" si="5"/>
         <v>1034.203880225049</v>
       </c>
-      <c r="X13" s="15">
+      <c r="X13" s="13">
         <f t="shared" si="6"/>
         <v>0.10580318375859296</v>
       </c>
-      <c r="Y13" s="16">
+      <c r="Y13" s="14">
         <f t="shared" si="7"/>
         <v>8.1997162763131737</v>
       </c>
-      <c r="Z13" s="17">
+      <c r="Z13" s="15">
         <f t="shared" si="8"/>
         <v>0.33797606075478032</v>
       </c>
-      <c r="AA13" s="18">
+      <c r="AA13" s="16">
         <f t="shared" si="9"/>
         <v>4.1909393274975413</v>
       </c>
-      <c r="AB13" s="18">
+      <c r="AB13" s="16">
         <f t="shared" si="0"/>
         <v>2.7939595516650271</v>
       </c>
-      <c r="AC13" s="18">
+      <c r="AC13" s="16">
         <f t="shared" si="10"/>
         <v>1.9956853940464481</v>
       </c>
-      <c r="AD13" s="17">
+      <c r="AD13" s="15">
         <f t="shared" si="11"/>
         <v>3.4249465648854964</v>
       </c>
-      <c r="AE13" s="12">
+      <c r="AE13" s="10">
         <f t="shared" si="12"/>
         <v>6.8498931297709929</v>
       </c>
-      <c r="AF13" s="18">
+      <c r="AF13" s="16">
         <f t="shared" si="13"/>
         <v>120.50779847328246</v>
       </c>
@@ -2684,12 +2684,12 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" s="4">
         <v>216000</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="12">
         <v>0</v>
       </c>
       <c r="J14" s="6">
@@ -2716,59 +2716,59 @@
       <c r="Q14" s="3">
         <v>190570.33306</v>
       </c>
-      <c r="S14" s="9">
+      <c r="S14" s="7">
         <f t="shared" si="1"/>
         <v>358.96118292579905</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="7">
         <f t="shared" si="2"/>
         <v>4.6473043835616439</v>
       </c>
-      <c r="U14" s="19">
+      <c r="U14" s="17">
         <f t="shared" si="3"/>
         <v>953.43290401323293</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V14" s="17">
         <f t="shared" si="4"/>
         <v>1794.8059146289952</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W14" s="17">
         <f t="shared" si="5"/>
         <v>1025.6033797879973</v>
       </c>
-      <c r="X14" s="15">
+      <c r="X14" s="13">
         <f t="shared" si="6"/>
         <v>0.11425171879549596</v>
       </c>
-      <c r="Y14" s="16">
+      <c r="Y14" s="14">
         <f t="shared" si="7"/>
         <v>4.6811231705725103</v>
       </c>
-      <c r="Z14" s="17">
+      <c r="Z14" s="15">
         <f t="shared" si="8"/>
         <v>0.26354537061852007</v>
       </c>
-      <c r="AA14" s="18">
+      <c r="AA14" s="16">
         <f t="shared" si="9"/>
         <v>4.7136015827921813</v>
       </c>
-      <c r="AB14" s="18">
+      <c r="AB14" s="16">
         <f t="shared" si="0"/>
         <v>3.142401055194787</v>
       </c>
-      <c r="AC14" s="18">
+      <c r="AC14" s="16">
         <f t="shared" si="10"/>
         <v>2.2445721822819911</v>
       </c>
-      <c r="AD14" s="17">
+      <c r="AD14" s="15">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AE14" s="12">
+      <c r="AE14" s="10">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AF14" s="18">
+      <c r="AF14" s="16">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -2793,12 +2793,12 @@
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H15" s="4">
         <v>83000</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="7">
         <v>8.6</v>
       </c>
       <c r="J15" s="6">
@@ -2825,59 +2825,59 @@
       <c r="Q15" s="3">
         <v>185978.81</v>
       </c>
-      <c r="S15" s="9">
+      <c r="S15" s="7">
         <f t="shared" si="1"/>
         <v>350.3561994714612</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="7">
         <f t="shared" si="2"/>
         <v>2.9733489041095891</v>
       </c>
-      <c r="U15" s="19">
+      <c r="U15" s="17">
         <f t="shared" si="3"/>
         <v>610.00710224991565</v>
       </c>
-      <c r="V15" s="19">
+      <c r="V15" s="17">
         <f t="shared" si="4"/>
         <v>1751.780997357306</v>
       </c>
-      <c r="W15" s="19">
+      <c r="W15" s="17">
         <f t="shared" si="5"/>
         <v>1001.0177127756035</v>
       </c>
-      <c r="X15" s="15">
+      <c r="X15" s="13">
         <f t="shared" si="6"/>
         <v>9.496599568941648E-2</v>
       </c>
-      <c r="Y15" s="16">
+      <c r="Y15" s="14">
         <f t="shared" si="7"/>
         <v>7.1402510930397636</v>
       </c>
-      <c r="Z15" s="17">
+      <c r="Z15" s="15">
         <f t="shared" si="8"/>
         <v>0.40204341674950839</v>
       </c>
-      <c r="AA15" s="18">
+      <c r="AA15" s="16">
         <f t="shared" si="9"/>
         <v>1.9979666438213535</v>
       </c>
-      <c r="AB15" s="18">
+      <c r="AB15" s="16">
         <f t="shared" si="0"/>
         <v>1.3319777625475691</v>
       </c>
-      <c r="AC15" s="18">
+      <c r="AC15" s="16">
         <f t="shared" si="10"/>
         <v>0.95141268753397779</v>
       </c>
-      <c r="AD15" s="17">
+      <c r="AD15" s="15">
         <f t="shared" si="11"/>
         <v>4.5134457831325303</v>
       </c>
-      <c r="AE15" s="12">
+      <c r="AE15" s="10">
         <f t="shared" si="12"/>
         <v>9.0268915662650606</v>
       </c>
-      <c r="AF15" s="18">
+      <c r="AF15" s="16">
         <f t="shared" si="13"/>
         <v>69.031267469879523</v>
       </c>
@@ -2902,12 +2902,12 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H16" s="4">
         <v>110000</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="7">
         <v>15.4</v>
       </c>
       <c r="J16" s="6">
@@ -2934,59 +2934,59 @@
       <c r="Q16" s="3">
         <v>331200.61</v>
       </c>
-      <c r="S16" s="9">
+      <c r="S16" s="7">
         <f t="shared" si="1"/>
         <v>325.56073846689497</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="7">
         <f t="shared" si="2"/>
         <v>2.009161728167808</v>
       </c>
-      <c r="U16" s="19">
+      <c r="U16" s="17">
         <f>T16/0.4*1000000/3412*0.35*0.8</f>
         <v>412.19613414931587</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V16" s="17">
         <f t="shared" si="4"/>
         <v>1627.8036923344748</v>
       </c>
-      <c r="W16" s="19">
+      <c r="W16" s="17">
         <f t="shared" si="5"/>
         <v>930.17353847684285</v>
       </c>
-      <c r="X16" s="15">
+      <c r="X16" s="13">
         <f t="shared" si="6"/>
         <v>8.4990327509480337E-2</v>
       </c>
-      <c r="Y16" s="16">
+      <c r="Y16" s="14">
         <f t="shared" si="7"/>
         <v>18.817941971880714</v>
       </c>
-      <c r="Z16" s="17">
+      <c r="Z16" s="15">
         <f t="shared" si="8"/>
         <v>0.55287397926995985</v>
       </c>
-      <c r="AA16" s="18">
+      <c r="AA16" s="16">
         <f t="shared" si="9"/>
         <v>2.0149849858714033</v>
       </c>
-      <c r="AB16" s="18">
+      <c r="AB16" s="16">
         <f t="shared" si="0"/>
         <v>1.3433233239142688</v>
       </c>
-      <c r="AC16" s="18">
+      <c r="AC16" s="16">
         <f t="shared" si="10"/>
         <v>0.95951665993876345</v>
       </c>
-      <c r="AD16" s="17">
+      <c r="AD16" s="15">
         <f t="shared" si="11"/>
         <v>6.0983999999999998</v>
       </c>
-      <c r="AE16" s="12">
+      <c r="AE16" s="10">
         <f t="shared" si="12"/>
         <v>12.1968</v>
       </c>
-      <c r="AF16" s="18">
+      <c r="AF16" s="16">
         <f t="shared" si="13"/>
         <v>172.43072000000001</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="4">
         <v>11684</v>
@@ -3019,8 +3019,8 @@
       <c r="I17" s="1">
         <v>4.5</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>68</v>
+      <c r="J17" s="18">
+        <v>3</v>
       </c>
       <c r="K17" s="4">
         <v>2412555.8387099998</v>
@@ -3043,59 +3043,59 @@
       <c r="Q17" s="3">
         <v>0</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S17" s="7">
         <f t="shared" si="1"/>
         <v>275.40591766095889</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U17" s="19">
+      <c r="U17" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V17" s="19">
+      <c r="V17" s="17">
         <f t="shared" si="4"/>
         <v>1377.0295883047943</v>
       </c>
-      <c r="W17" s="19">
+      <c r="W17" s="17">
         <f t="shared" si="5"/>
         <v>786.8740504598826</v>
       </c>
-      <c r="X17" s="15">
+      <c r="X17" s="13">
         <f t="shared" si="6"/>
         <v>8.3238659855175784E-2</v>
       </c>
-      <c r="Y17" s="16" t="e">
+      <c r="Y17" s="14" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Z17" s="17" t="e">
+      <c r="Z17" s="15" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA17" s="18">
+      <c r="AA17" s="16">
         <f t="shared" si="9"/>
         <v>1.8263950327284653</v>
       </c>
-      <c r="AB17" s="18">
+      <c r="AB17" s="16">
         <f t="shared" si="0"/>
         <v>1.2175966884856433</v>
       </c>
-      <c r="AC17" s="18">
+      <c r="AC17" s="16">
         <f t="shared" si="10"/>
         <v>0.86971192034688816</v>
       </c>
-      <c r="AD17" s="17">
+      <c r="AD17" s="15">
         <f t="shared" si="11"/>
         <v>16.776788770968846</v>
       </c>
-      <c r="AE17" s="12">
+      <c r="AE17" s="10">
         <f t="shared" si="12"/>
         <v>33.553577541937692</v>
       </c>
-      <c r="AF17" s="18">
+      <c r="AF17" s="16">
         <f t="shared" si="13"/>
         <v>146.4910989387196</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H18" s="4">
         <v>108000</v>
@@ -3152,59 +3152,59 @@
       <c r="Q18" s="3">
         <v>321118.34000000003</v>
       </c>
-      <c r="S18" s="9">
+      <c r="S18" s="7">
         <f t="shared" si="1"/>
         <v>252.38688252397259</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="7">
         <f t="shared" si="2"/>
         <v>2.2406238839326482</v>
       </c>
-      <c r="U18" s="19">
+      <c r="U18" s="17">
         <f t="shared" si="3"/>
         <v>459.68250842697944</v>
       </c>
-      <c r="V18" s="19">
+      <c r="V18" s="17">
         <f t="shared" si="4"/>
         <v>1261.9344126198628</v>
       </c>
-      <c r="W18" s="19">
+      <c r="W18" s="17">
         <f t="shared" si="5"/>
         <v>721.1053786399217</v>
       </c>
-      <c r="X18" s="15">
+      <c r="X18" s="13">
         <f t="shared" si="6"/>
         <v>0.11628845449912982</v>
       </c>
-      <c r="Y18" s="16">
+      <c r="Y18" s="14">
         <f t="shared" si="7"/>
         <v>16.360329375994613</v>
       </c>
-      <c r="Z18" s="17">
+      <c r="Z18" s="15">
         <f t="shared" si="8"/>
         <v>0.38433226091491568</v>
       </c>
-      <c r="AA18" s="18">
+      <c r="AA18" s="16">
         <f t="shared" si="9"/>
         <v>2.2940970394727409</v>
       </c>
-      <c r="AB18" s="18">
+      <c r="AB18" s="16">
         <f t="shared" si="0"/>
         <v>1.5293980263151605</v>
       </c>
-      <c r="AC18" s="18">
+      <c r="AC18" s="16">
         <f t="shared" si="10"/>
         <v>1.092427161653686</v>
       </c>
-      <c r="AD18" s="17">
+      <c r="AD18" s="15">
         <f t="shared" si="11"/>
         <v>8.6716666666666669</v>
       </c>
-      <c r="AE18" s="12">
+      <c r="AE18" s="10">
         <f t="shared" si="12"/>
         <v>17.343333333333334</v>
       </c>
-      <c r="AF18" s="18">
+      <c r="AF18" s="16">
         <f t="shared" si="13"/>
         <v>351.38166666666666</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" s="4">
         <v>191000</v>
@@ -3237,8 +3237,8 @@
       <c r="I19" s="1">
         <v>32.799999999999997</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>68</v>
+      <c r="J19" s="18">
+        <v>3</v>
       </c>
       <c r="K19" s="4">
         <v>2172835.0909099998</v>
@@ -3261,59 +3261,59 @@
       <c r="Q19" s="3">
         <v>67059.835449999999</v>
       </c>
-      <c r="S19" s="9">
+      <c r="S19" s="7">
         <f t="shared" si="1"/>
         <v>248.0405354920091</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="7">
         <f t="shared" si="2"/>
         <v>1.2530692203196347</v>
       </c>
-      <c r="U19" s="19">
+      <c r="U19" s="17">
         <f t="shared" si="3"/>
         <v>257.07750709957332</v>
       </c>
-      <c r="V19" s="19">
+      <c r="V19" s="17">
         <f t="shared" si="4"/>
         <v>1240.2026774600454</v>
       </c>
-      <c r="W19" s="19">
+      <c r="W19" s="17">
         <f t="shared" si="5"/>
         <v>708.68724426288315</v>
       </c>
-      <c r="X19" s="15">
+      <c r="X19" s="13">
         <f t="shared" si="6"/>
         <v>0.10637554178269382</v>
       </c>
-      <c r="Y19" s="16">
+      <c r="Y19" s="14">
         <f t="shared" si="7"/>
         <v>6.1091855367361338</v>
       </c>
-      <c r="Z19" s="17">
+      <c r="Z19" s="15">
         <f t="shared" si="8"/>
         <v>0.67539310149431009</v>
       </c>
-      <c r="AA19" s="18">
+      <c r="AA19" s="16">
         <f t="shared" si="9"/>
         <v>2.5116862401712989</v>
       </c>
-      <c r="AB19" s="18">
+      <c r="AB19" s="16">
         <f t="shared" si="0"/>
         <v>1.6744574934475327</v>
       </c>
-      <c r="AC19" s="18">
+      <c r="AC19" s="16">
         <f t="shared" si="10"/>
         <v>1.1960410667482375</v>
       </c>
-      <c r="AD19" s="17">
+      <c r="AD19" s="15">
         <f t="shared" si="11"/>
         <v>7.4804607329842918</v>
       </c>
-      <c r="AE19" s="12">
+      <c r="AE19" s="10">
         <f t="shared" si="12"/>
         <v>14.960921465968584</v>
       </c>
-      <c r="AF19" s="18">
+      <c r="AF19" s="16">
         <f t="shared" si="13"/>
         <v>457.91822408376953</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="4">
         <v>66500</v>
@@ -3346,8 +3346,8 @@
       <c r="I20" s="1">
         <v>81.260000000000005</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>139</v>
+      <c r="J20" s="18">
+        <v>2</v>
       </c>
       <c r="K20" s="4">
         <v>2132806.05339</v>
@@ -3371,61 +3371,61 @@
         <v>148312.74807</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="S20" s="9">
+        <v>146</v>
+      </c>
+      <c r="S20" s="7">
         <f t="shared" si="1"/>
         <v>243.47101066095891</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="7">
         <f t="shared" si="2"/>
         <v>3.5778371267123288</v>
       </c>
-      <c r="U20" s="19">
+      <c r="U20" s="17">
         <f t="shared" si="3"/>
         <v>734.02285718013763</v>
       </c>
-      <c r="V20" s="19">
+      <c r="V20" s="17">
         <f t="shared" si="4"/>
         <v>1217.3550533047944</v>
       </c>
-      <c r="W20" s="19">
+      <c r="W20" s="17">
         <f t="shared" si="5"/>
         <v>695.63145903131124</v>
       </c>
-      <c r="X20" s="15">
+      <c r="X20" s="13">
         <f t="shared" si="6"/>
         <v>0.10656346290313171</v>
       </c>
-      <c r="Y20" s="16">
+      <c r="Y20" s="14">
         <f t="shared" si="7"/>
         <v>4.7320988641487549</v>
       </c>
-      <c r="Z20" s="17">
+      <c r="Z20" s="15">
         <f t="shared" si="8"/>
         <v>0.23218583153854813</v>
       </c>
-      <c r="AA20" s="18">
+      <c r="AA20" s="16">
         <f t="shared" si="9"/>
         <v>2.332926611911748</v>
       </c>
-      <c r="AB20" s="18">
+      <c r="AB20" s="16">
         <f t="shared" si="0"/>
         <v>1.5552844079411654</v>
       </c>
-      <c r="AC20" s="18">
+      <c r="AC20" s="16">
         <f t="shared" si="10"/>
         <v>1.1109174342436896</v>
       </c>
-      <c r="AD20" s="17">
+      <c r="AD20" s="15">
         <f t="shared" si="11"/>
         <v>53.228354887218046</v>
       </c>
-      <c r="AE20" s="12">
+      <c r="AE20" s="10">
         <f t="shared" si="12"/>
         <v>106.45670977443609</v>
       </c>
-      <c r="AF20" s="18">
+      <c r="AF20" s="16">
         <f t="shared" si="13"/>
         <v>8569.4122362706767</v>
       </c>
@@ -3450,12 +3450,12 @@
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H21" s="4">
         <v>133000</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="7">
         <v>14.2</v>
       </c>
       <c r="J21" s="6">
@@ -3482,59 +3482,59 @@
       <c r="Q21" s="3">
         <v>91811.24</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S21" s="7">
         <f t="shared" si="1"/>
         <v>227.44800401255708</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="7">
         <f t="shared" si="2"/>
         <v>1.3325923515981735</v>
       </c>
-      <c r="U21" s="19">
+      <c r="U21" s="17">
         <f t="shared" si="3"/>
         <v>273.39233473585034</v>
       </c>
-      <c r="V21" s="19">
+      <c r="V21" s="17">
         <f t="shared" si="4"/>
         <v>1137.2400200627853</v>
       </c>
-      <c r="W21" s="19">
+      <c r="W21" s="17">
         <f t="shared" si="5"/>
         <v>649.85144003587743</v>
       </c>
-      <c r="X21" s="15">
+      <c r="X21" s="13">
         <f t="shared" si="6"/>
         <v>9.3864719608475658E-2</v>
       </c>
-      <c r="Y21" s="16">
+      <c r="Y21" s="14">
         <f t="shared" si="7"/>
         <v>7.8649221926329096</v>
       </c>
-      <c r="Z21" s="17">
+      <c r="Z21" s="15">
         <f t="shared" si="8"/>
         <v>0.5823630825736974</v>
       </c>
-      <c r="AA21" s="18">
+      <c r="AA21" s="16">
         <f t="shared" si="9"/>
         <v>1.8421792788160392</v>
       </c>
-      <c r="AB21" s="18">
+      <c r="AB21" s="16">
         <f t="shared" si="0"/>
         <v>1.2281195192106926</v>
       </c>
-      <c r="AC21" s="18">
+      <c r="AC21" s="16">
         <f t="shared" si="10"/>
         <v>0.87722822800763767</v>
       </c>
-      <c r="AD21" s="17">
+      <c r="AD21" s="15">
         <f t="shared" si="11"/>
         <v>4.6507669172932333</v>
       </c>
-      <c r="AE21" s="12">
+      <c r="AE21" s="10">
         <f t="shared" si="12"/>
         <v>9.3015338345864667</v>
       </c>
-      <c r="AF21" s="18">
+      <c r="AF21" s="16">
         <f t="shared" si="13"/>
         <v>117.88178045112782</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" s="4">
         <v>8078</v>
@@ -3567,8 +3567,8 @@
       <c r="I22" s="1">
         <v>0.76</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>68</v>
+      <c r="J22" s="18">
+        <v>3</v>
       </c>
       <c r="K22" s="4">
         <v>1722688.44414</v>
@@ -3591,59 +3591,59 @@
       <c r="Q22" s="3">
         <v>1144.9751699999999</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S22" s="7">
         <f t="shared" si="1"/>
         <v>196.65393197945207</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="7">
         <f t="shared" si="2"/>
         <v>1.3011769406392693E-2</v>
       </c>
-      <c r="U22" s="19">
+      <c r="U22" s="17">
         <f t="shared" si="3"/>
         <v>2.6694720353091697</v>
       </c>
-      <c r="V22" s="19">
+      <c r="V22" s="17">
         <f t="shared" si="4"/>
         <v>983.26965989726034</v>
       </c>
-      <c r="W22" s="19">
+      <c r="W22" s="17">
         <f t="shared" si="5"/>
         <v>561.86837708414885</v>
       </c>
-      <c r="X22" s="15">
+      <c r="X22" s="13">
         <f t="shared" si="6"/>
         <v>8.9124068819447316E-2</v>
       </c>
-      <c r="Y22" s="16">
+      <c r="Y22" s="14">
         <f t="shared" si="7"/>
         <v>10.045130988716748</v>
       </c>
-      <c r="Z22" s="17">
+      <c r="Z22" s="15">
         <f t="shared" si="8"/>
         <v>51.567407549063674</v>
       </c>
-      <c r="AA22" s="18">
+      <c r="AA22" s="16">
         <f t="shared" si="9"/>
         <v>1.2102478582775964</v>
       </c>
-      <c r="AB22" s="18">
+      <c r="AB22" s="16">
         <f t="shared" si="0"/>
         <v>0.80683190551839767</v>
       </c>
-      <c r="AC22" s="18">
+      <c r="AC22" s="16">
         <f t="shared" si="10"/>
         <v>0.57630850394171262</v>
       </c>
-      <c r="AD22" s="17">
+      <c r="AD22" s="15">
         <f t="shared" si="11"/>
         <v>4.0982421391433519</v>
       </c>
-      <c r="AE22" s="12">
+      <c r="AE22" s="10">
         <f t="shared" si="12"/>
         <v>8.1964842782867038</v>
       </c>
-      <c r="AF22" s="18">
+      <c r="AF22" s="16">
         <f t="shared" si="13"/>
         <v>5.4693280514978948</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="4">
         <v>115000</v>
@@ -3676,8 +3676,8 @@
       <c r="I23" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>139</v>
+      <c r="J23" s="18">
+        <v>2</v>
       </c>
       <c r="K23" s="4">
         <v>1436221.7472399999</v>
@@ -3700,59 +3700,59 @@
       <c r="Q23" s="3">
         <v>73902.525169999994</v>
       </c>
-      <c r="S23" s="9">
+      <c r="S23" s="7">
         <f t="shared" si="1"/>
         <v>163.95225425114154</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="7">
         <f t="shared" si="2"/>
         <v>1.279188084474886</v>
       </c>
-      <c r="U23" s="19">
+      <c r="U23" s="17">
         <f t="shared" si="3"/>
         <v>262.43600795205742</v>
       </c>
-      <c r="V23" s="19">
+      <c r="V23" s="17">
         <f t="shared" si="4"/>
         <v>819.7612712557077</v>
       </c>
-      <c r="W23" s="19">
+      <c r="W23" s="17">
         <f t="shared" si="5"/>
         <v>468.43501214611871</v>
       </c>
-      <c r="X23" s="15">
+      <c r="X23" s="13">
         <f t="shared" si="6"/>
         <v>0.14298596895962709</v>
       </c>
-      <c r="Y23" s="16">
+      <c r="Y23" s="14">
         <f t="shared" si="7"/>
         <v>6.5950906072107687</v>
       </c>
-      <c r="Z23" s="17">
+      <c r="Z23" s="15">
         <f t="shared" si="8"/>
         <v>0.43731261907003616</v>
       </c>
-      <c r="AA23" s="18">
+      <c r="AA23" s="16">
         <f t="shared" si="9"/>
         <v>4.5501051718220333</v>
       </c>
-      <c r="AB23" s="18">
+      <c r="AB23" s="16">
         <f t="shared" si="0"/>
         <v>3.0334034478813554</v>
       </c>
-      <c r="AC23" s="18">
+      <c r="AC23" s="16">
         <f t="shared" si="10"/>
         <v>2.1667167484866821</v>
       </c>
-      <c r="AD23" s="17">
+      <c r="AD23" s="15">
         <f t="shared" si="11"/>
         <v>3.7120695652173916</v>
       </c>
-      <c r="AE23" s="12">
+      <c r="AE23" s="10">
         <f t="shared" si="12"/>
         <v>7.4241391304347832</v>
       </c>
-      <c r="AF23" s="18">
+      <c r="AF23" s="16">
         <f t="shared" si="13"/>
         <v>62.956563478260883</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H24" s="4">
         <v>108000</v>
@@ -3809,59 +3809,59 @@
       <c r="Q24" s="3">
         <v>4930</v>
       </c>
-      <c r="S24" s="9">
+      <c r="S24" s="7">
         <f t="shared" si="1"/>
         <v>79.250570776255714</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="7">
         <f t="shared" si="2"/>
         <v>5.9589041095890409E-2</v>
       </c>
-      <c r="U24" s="19">
+      <c r="U24" s="17">
         <f t="shared" si="3"/>
         <v>12.225184281102955</v>
       </c>
-      <c r="V24" s="19">
+      <c r="V24" s="17">
         <f t="shared" si="4"/>
         <v>396.25285388127855</v>
       </c>
-      <c r="W24" s="19">
+      <c r="W24" s="17">
         <f t="shared" si="5"/>
         <v>226.43020221787347</v>
       </c>
-      <c r="X24" s="15">
+      <c r="X24" s="13">
         <f t="shared" si="6"/>
         <v>0.1595338754168257</v>
       </c>
-      <c r="Y24" s="16">
+      <c r="Y24" s="14">
         <f t="shared" si="7"/>
         <v>9.4444444444444446</v>
       </c>
-      <c r="Z24" s="17">
+      <c r="Z24" s="15">
         <f t="shared" si="8"/>
         <v>4.5377965900383144</v>
       </c>
-      <c r="AA24" s="18">
+      <c r="AA24" s="16">
         <f t="shared" si="9"/>
         <v>3.3312062918176117</v>
       </c>
-      <c r="AB24" s="18">
+      <c r="AB24" s="16">
         <f t="shared" si="0"/>
         <v>2.2208041945450745</v>
       </c>
-      <c r="AC24" s="18">
+      <c r="AC24" s="16">
         <f t="shared" si="10"/>
         <v>1.5862887103893388</v>
       </c>
-      <c r="AD24" s="17">
+      <c r="AD24" s="15">
         <f t="shared" si="11"/>
         <v>2.7426666666666666</v>
       </c>
-      <c r="AE24" s="12">
+      <c r="AE24" s="10">
         <f t="shared" si="12"/>
         <v>5.4853333333333332</v>
       </c>
-      <c r="AF24" s="18">
+      <c r="AF24" s="16">
         <f t="shared" si="13"/>
         <v>30.500266666666665</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H25" s="4">
         <v>239260</v>
@@ -3921,59 +3921,59 @@
       <c r="R25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="S25" s="9">
+      <c r="S25" s="7">
         <f t="shared" si="1"/>
         <v>508.1784851598174</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="7">
         <f t="shared" si="2"/>
         <v>0.22517123287671234</v>
       </c>
-      <c r="U25" s="19">
+      <c r="U25" s="17">
         <f t="shared" si="3"/>
         <v>46.195739453018348</v>
       </c>
-      <c r="V25" s="19">
+      <c r="V25" s="17">
         <f t="shared" si="4"/>
         <v>2540.8924257990871</v>
       </c>
-      <c r="W25" s="19">
+      <c r="W25" s="17">
         <f t="shared" si="5"/>
         <v>1451.9385290280497</v>
       </c>
-      <c r="X25" s="15">
+      <c r="X25" s="13">
         <f t="shared" si="6"/>
         <v>0.10787846258660337</v>
       </c>
-      <c r="Y25" s="16">
+      <c r="Y25" s="14">
         <f t="shared" si="7"/>
         <v>11.164238276299113</v>
       </c>
-      <c r="Z25" s="17">
+      <c r="Z25" s="15">
         <f t="shared" si="8"/>
         <v>7.7003841441622303</v>
       </c>
-      <c r="AA25" s="18" t="e">
+      <c r="AA25" s="16" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB25" s="18" t="e">
+      <c r="AB25" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC25" s="18" t="e">
+      <c r="AC25" s="16" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD25" s="17">
+      <c r="AD25" s="15">
         <f t="shared" si="11"/>
         <v>5.316191590738109</v>
       </c>
-      <c r="AE25" s="12">
+      <c r="AE25" s="10">
         <f t="shared" si="12"/>
         <v>10.632383181476218</v>
       </c>
-      <c r="AF25" s="18">
+      <c r="AF25" s="16">
         <f t="shared" si="13"/>
         <v>281.26558889910558</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" s="4">
         <v>236874</v>
@@ -4033,59 +4033,59 @@
       <c r="R26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="S26" s="9">
+      <c r="S26" s="7">
         <f t="shared" si="1"/>
         <v>435.55773858447486</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="7">
         <f t="shared" si="2"/>
         <v>5.3645205479452054</v>
       </c>
-      <c r="U26" s="19">
+      <c r="U26" s="17">
         <f t="shared" si="3"/>
         <v>1100.5757278902825</v>
       </c>
-      <c r="V26" s="19">
+      <c r="V26" s="17">
         <f t="shared" si="4"/>
         <v>2177.7886929223741</v>
       </c>
-      <c r="W26" s="19">
+      <c r="W26" s="17">
         <f t="shared" si="5"/>
         <v>1244.4506816699281</v>
       </c>
-      <c r="X26" s="15">
+      <c r="X26" s="13">
         <f t="shared" si="6"/>
         <v>8.4036950377424938E-2</v>
       </c>
-      <c r="Y26" s="16">
+      <c r="Y26" s="14">
         <f t="shared" si="7"/>
         <v>1.0535005064562533</v>
       </c>
-      <c r="Z26" s="17">
+      <c r="Z26" s="15">
         <f t="shared" si="8"/>
         <v>0.27702811290739937</v>
       </c>
-      <c r="AA26" s="18" t="e">
+      <c r="AA26" s="16" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB26" s="18" t="e">
+      <c r="AB26" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC26" s="18" t="e">
+      <c r="AC26" s="16" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD26" s="17">
+      <c r="AD26" s="15">
         <f t="shared" si="11"/>
         <v>4.4502646976873779</v>
       </c>
-      <c r="AE26" s="12">
+      <c r="AE26" s="10">
         <f t="shared" si="12"/>
         <v>8.9005293953747557</v>
       </c>
-      <c r="AF26" s="18">
+      <c r="AF26" s="16">
         <f t="shared" si="13"/>
         <v>191.19281136806907</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
         <v>134</v>
@@ -4110,7 +4110,7 @@
         <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H27" s="4">
         <v>93750</v>
@@ -4145,59 +4145,59 @@
       <c r="R27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="S27" s="9">
+      <c r="S27" s="7">
         <f t="shared" si="1"/>
         <v>69.59838127853881</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="7">
         <f t="shared" si="2"/>
         <v>0.42234018264840179</v>
       </c>
-      <c r="U27" s="19">
+      <c r="U27" s="17">
         <f t="shared" si="3"/>
         <v>86.646579089648654</v>
       </c>
-      <c r="V27" s="19">
+      <c r="V27" s="17">
         <f t="shared" si="4"/>
         <v>347.99190639269403</v>
       </c>
-      <c r="W27" s="19">
+      <c r="W27" s="17">
         <f t="shared" si="5"/>
         <v>198.85251793868233</v>
       </c>
-      <c r="X27" s="15">
+      <c r="X27" s="13">
         <f t="shared" si="6"/>
         <v>0.11903889474677137</v>
       </c>
-      <c r="Y27" s="16">
+      <c r="Y27" s="14">
         <f t="shared" si="7"/>
         <v>11.101778522582913</v>
       </c>
-      <c r="Z27" s="17">
+      <c r="Z27" s="15">
         <f t="shared" si="8"/>
         <v>0.56227109491039806</v>
       </c>
-      <c r="AA27" s="18" t="e">
+      <c r="AA27" s="16" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB27" s="18" t="e">
+      <c r="AB27" s="16" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC27" s="18" t="e">
+      <c r="AC27" s="16" t="e">
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD27" s="17">
+      <c r="AD27" s="15">
         <f t="shared" si="11"/>
         <v>1.8120959999999999</v>
       </c>
-      <c r="AE27" s="12">
+      <c r="AE27" s="10">
         <f t="shared" si="12"/>
         <v>3.6241919999999999</v>
       </c>
-      <c r="AF27" s="18">
+      <c r="AF27" s="16">
         <f t="shared" si="13"/>
         <v>10.234348799999999</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H28" s="4">
         <v>844480</v>
@@ -4230,8 +4230,8 @@
       <c r="I28" s="1">
         <v>49.1</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>68</v>
+      <c r="J28" s="18">
+        <v>3</v>
       </c>
       <c r="K28" s="4">
         <v>559000</v>
@@ -4257,59 +4257,59 @@
       <c r="R28" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="S28" s="9">
+      <c r="S28" s="7">
         <f t="shared" si="1"/>
         <v>63.812785388127857</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28" s="7">
         <f t="shared" si="2"/>
         <v>0.17992009132420089</v>
       </c>
-      <c r="U28" s="19">
+      <c r="U28" s="17">
         <f t="shared" si="3"/>
         <v>36.912093765222927</v>
       </c>
-      <c r="V28" s="19">
+      <c r="V28" s="17">
         <f t="shared" si="4"/>
         <v>319.06392694063925</v>
       </c>
-      <c r="W28" s="19">
+      <c r="W28" s="17">
         <f t="shared" si="5"/>
         <v>182.32224396607961</v>
       </c>
-      <c r="X28" s="15">
+      <c r="X28" s="13">
         <f t="shared" si="6"/>
         <v>0.13956148479427549</v>
       </c>
-      <c r="Y28" s="16">
+      <c r="Y28" s="14">
         <f t="shared" si="7"/>
         <v>7.7792525854958443</v>
       </c>
-      <c r="Z28" s="17">
+      <c r="Z28" s="15">
         <f t="shared" si="8"/>
         <v>1.2101440263942642</v>
       </c>
-      <c r="AA28" s="18">
+      <c r="AA28" s="16">
         <f t="shared" si="9"/>
         <v>6.205652951699463</v>
       </c>
-      <c r="AB28" s="18">
+      <c r="AB28" s="16">
         <f t="shared" si="0"/>
         <v>4.1371019677996417</v>
       </c>
-      <c r="AC28" s="18">
+      <c r="AC28" s="16">
         <f t="shared" si="10"/>
         <v>2.9550728341426011</v>
       </c>
-      <c r="AD28" s="17">
+      <c r="AD28" s="15">
         <f t="shared" si="11"/>
         <v>2.5326780977643049</v>
       </c>
-      <c r="AE28" s="12">
+      <c r="AE28" s="10">
         <f t="shared" si="12"/>
         <v>5.0653561955286097</v>
       </c>
-      <c r="AF28" s="18">
+      <c r="AF28" s="16">
         <f t="shared" si="13"/>
         <v>199.60898920045474</v>
       </c>
@@ -4327,39 +4327,42 @@
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>178</v>
+      <c r="A32" s="11" t="s">
+        <v>177</v>
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>178</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>179</v>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>181</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>181</v>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4371,6 +4374,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78ce7efe-c353-4cf8-9d4c-148e26a147e3" xsi:nil="true"/>
+    <Dataextractedfrom50statebiogasprofilesinpdf xmlns="65950468-3135-4891-ae74-8a1589473272" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65950468-3135-4891-ae74-8a1589473272">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EA8C0B3A98985478596F957EEE5A42B" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="813a874e57bc7ee77ed2d675827f2fdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65950468-3135-4891-ae74-8a1589473272" xmlns:ns3="78ce7efe-c353-4cf8-9d4c-148e26a147e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52589cb147cfc41901144a84263f1621" ns2:_="" ns3:_="">
     <xsd:import namespace="65950468-3135-4891-ae74-8a1589473272"/>
@@ -4597,28 +4621,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE0FBAF-579E-429E-B254-9759185C8EB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="65950468-3135-4891-ae74-8a1589473272"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="78ce7efe-c353-4cf8-9d4c-148e26a147e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78ce7efe-c353-4cf8-9d4c-148e26a147e3" xsi:nil="true"/>
-    <Dataextractedfrom50statebiogasprofilesinpdf xmlns="65950468-3135-4891-ae74-8a1589473272" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65950468-3135-4891-ae74-8a1589473272">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D085DC7-2B76-4A87-9F5C-038FAA97CFCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47952F0A-656C-49A9-873F-B128AEF0E2E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4635,29 +4663,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D085DC7-2B76-4A87-9F5C-038FAA97CFCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE0FBAF-579E-429E-B254-9759185C8EB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="65950468-3135-4891-ae74-8a1589473272"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="78ce7efe-c353-4cf8-9d4c-148e26a147e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates and finish results for PV Wind and CHP
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbecker\JuliaPlay\oshkosh-portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbecker\GitHub\oshkosh-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55659669-EC85-441B-A417-737B392A93A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF42DFC-A5E4-45DF-8C03-DFF8D38B7A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2145" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OshKosh Locations by TAP" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="State NEM Policies" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'OshKosh Data'!$A$1:$AJ$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'OshKosh Data'!$A$1:$AK$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'State NEM Policies'!$K$1:$V$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="306">
   <si>
     <t>City</t>
   </si>
@@ -1491,9 +1491,6 @@
     <t>Done?</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>TBD</t>
   </si>
   <si>
@@ -1503,9 +1500,6 @@
     <t>Cooling Load Annual Ton-Hr</t>
   </si>
   <si>
-    <t>Cooling too high</t>
-  </si>
-  <si>
     <t>Site Number</t>
   </si>
   <si>
@@ -1513,13 +1507,16 @@
   </si>
   <si>
     <t>cents/kWh</t>
+  </si>
+  <si>
+    <t>Heat/Cool Ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1527,6 +1524,7 @@
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00000"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1670,7 +1668,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1767,11 +1765,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2153,7 +2155,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'OshKosh Data'!$AM$2:$AM$28</c:f>
+              <c:f>'OshKosh Data'!$AN$2:$AN$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -2227,7 +2229,7 @@
                   <c:v>13.098411729753167</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>6.5993913504304669E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1415.0259358589346</c:v>
@@ -2776,7 +2778,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'OshKosh Data'!$AN$2:$AN$28</c:f>
+              <c:f>'OshKosh Data'!$AO$2:$AO$28</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="27"/>
@@ -6129,8 +6131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2:AL28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6164,8 +6166,9 @@
     <col min="28" max="28" width="14.28515625" customWidth="1"/>
     <col min="29" max="31" width="15" style="1" customWidth="1"/>
     <col min="33" max="35" width="15" style="1" customWidth="1"/>
-    <col min="36" max="36" width="16.28515625" customWidth="1"/>
-    <col min="41" max="43" width="12.7109375" customWidth="1"/>
+    <col min="36" max="36" width="12.7109375" customWidth="1"/>
+    <col min="37" max="37" width="16.28515625" customWidth="1"/>
+    <col min="42" max="43" width="12.7109375" customWidth="1"/>
     <col min="44" max="44" width="11.85546875" customWidth="1"/>
     <col min="45" max="45" width="12.7109375" customWidth="1"/>
   </cols>
@@ -6250,7 +6253,7 @@
         <v>293</v>
       </c>
       <c r="AA1" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AB1" s="11" t="s">
         <v>291</v>
@@ -6265,7 +6268,7 @@
         <v>292</v>
       </c>
       <c r="AF1" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>290</v>
@@ -6277,21 +6280,23 @@
         <v>289</v>
       </c>
       <c r="AJ1" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK1" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="AK1" s="22" t="s">
+      <c r="AL1" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="AM1" s="11" t="s">
-        <v>305</v>
-      </c>
       <c r="AN1" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="AO1" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>304</v>
+      </c>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
@@ -6409,25 +6414,28 @@
         <f>MIN(Z2/0.35,(I2-H2/43560)/30*1000)</f>
         <v>2806.588613406795</v>
       </c>
-      <c r="AJ2" s="43">
-        <f>AC2*3412/1000000*Y2-K2/2.5*X2</f>
-        <v>-568026.60938103439</v>
-      </c>
-      <c r="AK2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL2" t="s">
+      <c r="AJ2" s="45">
+        <f>AC2*1000000/3412/(AA2*3.51)</f>
+        <v>39.879303805855251</v>
+      </c>
+      <c r="AK2" s="43">
+        <f>AC2*Y2+AA2*3.52/(6-4)*X2-AC2*1000000/3412/4*X2</f>
+        <v>179482.32815609896</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM2">
-        <f t="shared" ref="AM2:AM28" si="4">AD2*1000000/3412</f>
+      <c r="AN2">
+        <f t="shared" ref="AN2:AN28" si="4">AD2*1000000/3412</f>
         <v>3132.408712953074</v>
       </c>
-      <c r="AN2" s="20">
+      <c r="AO2" s="20">
         <f>X2*100</f>
         <v>7.8293532609545231</v>
       </c>
-      <c r="AO2" s="46"/>
     </row>
     <row r="3" spans="1:45" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -6546,22 +6554,26 @@
         <f t="shared" ref="AI3:AI28" si="11">MIN(Z3/0.35,(I3-H3/43560)/30*1000)</f>
         <v>1090.016069788797</v>
       </c>
-      <c r="AJ3" s="43">
-        <f t="shared" ref="AJ3:AJ28" si="12">AC3*3412/1000000*Y3-K3/2.5*X3</f>
-        <v>-492376.49237871886</v>
-      </c>
-      <c r="AK3" t="b">
+      <c r="AJ3" s="45">
+        <f>AC3*1000000/3412/(AA3*3.51)</f>
+        <v>28.983439292896232</v>
+      </c>
+      <c r="AK3" s="43">
+        <f t="shared" ref="AK3:AK28" si="12">AC3*Y3+AA3*3.52/(6-4)*X3-AC3*1000000/3412/4*X3</f>
+        <v>-210935.91546570824</v>
+      </c>
+      <c r="AL3" t="b">
         <v>1</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <f t="shared" si="4"/>
         <v>2823.392100536918</v>
       </c>
-      <c r="AN3" s="20">
-        <f t="shared" ref="AN3:AN28" si="13">X3*100</f>
+      <c r="AO3" s="20">
+        <f t="shared" ref="AO3:AO28" si="13">X3*100</f>
         <v>10.801228474600522</v>
       </c>
     </row>
@@ -6679,21 +6691,25 @@
         <f t="shared" si="11"/>
         <v>1308.4144475053567</v>
       </c>
-      <c r="AJ4" s="43">
+      <c r="AJ4" s="45" t="e">
+        <f>AC4*1000000/3412/(AA4*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK4" s="43">
         <f t="shared" si="12"/>
-        <v>-292954.85629391362</v>
-      </c>
-      <c r="AK4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL4" t="s">
+        <v>-124218.5160676708</v>
+      </c>
+      <c r="AL4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <f t="shared" si="4"/>
         <v>1067.3524814380617</v>
       </c>
-      <c r="AN4" s="20">
+      <c r="AO4" s="20">
         <f t="shared" si="13"/>
         <v>11.687476243467355</v>
       </c>
@@ -6813,21 +6829,25 @@
         <f t="shared" si="11"/>
         <v>1737.5971839608203</v>
       </c>
-      <c r="AJ5" s="43">
+      <c r="AJ5" s="45">
+        <f>AC5*1000000/3412/(AA5*3.51)</f>
+        <v>8.0935616245483982E-2</v>
+      </c>
+      <c r="AK5" s="43">
         <f t="shared" si="12"/>
-        <v>-336788.90180921968</v>
-      </c>
-      <c r="AK5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="s">
+        <v>249298.92548384395</v>
+      </c>
+      <c r="AL5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <f t="shared" si="4"/>
         <v>59.219582577205358</v>
       </c>
-      <c r="AN5" s="20">
+      <c r="AO5" s="20">
         <f t="shared" si="13"/>
         <v>7.1081033409441332</v>
       </c>
@@ -6946,21 +6966,25 @@
         <f t="shared" si="11"/>
         <v>3768.3197323352906</v>
       </c>
-      <c r="AJ6" s="43">
+      <c r="AJ6" s="45" t="e">
+        <f>AC6*1000000/3412/(AA6*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK6" s="43">
         <f t="shared" si="12"/>
-        <v>-600900.54254894156</v>
-      </c>
-      <c r="AK6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="s">
+        <v>-145523.58164540294</v>
+      </c>
+      <c r="AL6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <f t="shared" si="4"/>
         <v>3845.758964375666</v>
       </c>
-      <c r="AN6" s="20">
+      <c r="AO6" s="20">
         <f t="shared" si="13"/>
         <v>13.07292003671493</v>
       </c>
@@ -6973,7 +6997,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D7" t="s">
         <v>105</v>
@@ -7082,21 +7106,25 @@
         <f t="shared" si="11"/>
         <v>2336.7658402203861</v>
       </c>
-      <c r="AJ7" s="43">
+      <c r="AJ7" s="45">
+        <f>AC7*1000000/3412/(AA7*3.51)</f>
+        <v>104.59443090663524</v>
+      </c>
+      <c r="AK7" s="43">
         <f t="shared" si="12"/>
-        <v>-368634.97063979111</v>
-      </c>
-      <c r="AK7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL7" t="s">
+        <v>-207750.97062046407</v>
+      </c>
+      <c r="AL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM7" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <f t="shared" si="4"/>
         <v>4120.4198460008192</v>
       </c>
-      <c r="AN7" s="20">
+      <c r="AO7" s="20">
         <f t="shared" si="13"/>
         <v>8.4001571950601353</v>
       </c>
@@ -7218,21 +7246,25 @@
         <f t="shared" si="11"/>
         <v>2176.2027598695367</v>
       </c>
-      <c r="AJ8" s="43">
-        <f t="shared" si="12"/>
-        <v>-312234.14264039003</v>
-      </c>
-      <c r="AK8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL8" t="s">
+      <c r="AJ8" s="46">
+        <f>AC8*1000000/3412/(AA8*3.51)</f>
+        <v>1.2710437928260929</v>
+      </c>
+      <c r="AK8" s="47">
+        <f>AC8*Y8+AA8*3.52/(6-4)*X8-AC8*1000000/3412/4*X8</f>
+        <v>189837.72719522053</v>
+      </c>
+      <c r="AL8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <f t="shared" si="4"/>
         <v>446.47064918605838</v>
       </c>
-      <c r="AN8" s="20">
+      <c r="AO8" s="20">
         <f t="shared" si="13"/>
         <v>11.714809607723407</v>
       </c>
@@ -7351,21 +7383,25 @@
         <f t="shared" si="11"/>
         <v>289.45821854912765</v>
       </c>
-      <c r="AJ9" s="43">
+      <c r="AJ9" s="45">
+        <f>AC9*1000000/3412/(AA9*3.51)</f>
+        <v>14.495245566075182</v>
+      </c>
+      <c r="AK9" s="43">
         <f t="shared" si="12"/>
-        <v>-208625.03273801095</v>
-      </c>
-      <c r="AK9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL9" t="s">
+        <v>-12597.367698121438</v>
+      </c>
+      <c r="AL9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <f t="shared" si="4"/>
         <v>571.02942274647103</v>
       </c>
-      <c r="AN9" s="20">
+      <c r="AO9" s="20">
         <f t="shared" si="13"/>
         <v>10.588080890888051</v>
       </c>
@@ -7478,21 +7514,25 @@
         <f t="shared" si="11"/>
         <v>866.84266911539635</v>
       </c>
-      <c r="AJ10" s="43">
+      <c r="AJ10" s="46">
+        <f>AC10*1000000/3412/(AA10*3.51)</f>
+        <v>1.0250367183516813</v>
+      </c>
+      <c r="AK10" s="47">
         <f t="shared" si="12"/>
-        <v>-203283.07785021313</v>
-      </c>
-      <c r="AK10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL10" t="s">
+        <v>73981.12509801492</v>
+      </c>
+      <c r="AL10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <f t="shared" si="4"/>
         <v>171.99209357786378</v>
       </c>
-      <c r="AN10" s="20">
+      <c r="AO10" s="20">
         <f t="shared" si="13"/>
         <v>10.489337687527119</v>
       </c>
@@ -7611,21 +7651,25 @@
         <f t="shared" si="11"/>
         <v>958.90113253749632</v>
       </c>
-      <c r="AJ11" s="43">
+      <c r="AJ11" s="45">
+        <f>AC11*1000000/3412/(AA11*3.51)</f>
+        <v>208.86838967315506</v>
+      </c>
+      <c r="AK11" s="43">
         <f t="shared" si="12"/>
-        <v>-153709.70440728177</v>
-      </c>
-      <c r="AK11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL11" t="s">
+        <v>-62038.503897735645</v>
+      </c>
+      <c r="AL11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <f t="shared" si="4"/>
         <v>910.9973948513707</v>
       </c>
-      <c r="AN11" s="20">
+      <c r="AO11" s="20">
         <f t="shared" si="13"/>
         <v>9.9339549469953106</v>
       </c>
@@ -7710,7 +7754,7 @@
         <f t="shared" si="5"/>
         <v>367.84281674429224</v>
       </c>
-      <c r="AA12" s="45">
+      <c r="AA12" s="44">
         <f>U12*4*3.52/((4.4+4.69)/2)</f>
         <v>221680.61590154769</v>
       </c>
@@ -7745,21 +7789,25 @@
         <f t="shared" si="11"/>
         <v>1050.9794764122637</v>
       </c>
-      <c r="AJ12" s="43">
+      <c r="AJ12" s="46">
+        <f>AC12*1000000/3412/(AA12*3.51)</f>
+        <v>2.8596001086341993</v>
+      </c>
+      <c r="AK12" s="47">
         <f t="shared" si="12"/>
-        <v>-110387.88597975999</v>
-      </c>
-      <c r="AK12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="44" t="s">
-        <v>303</v>
-      </c>
-      <c r="AM12">
+        <v>88746.880483559391</v>
+      </c>
+      <c r="AL12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN12">
         <f t="shared" si="4"/>
         <v>254.00135567724979</v>
       </c>
-      <c r="AN12" s="20">
+      <c r="AO12" s="20">
         <f t="shared" si="13"/>
         <v>8.5916331345552663</v>
       </c>
@@ -7878,21 +7926,25 @@
         <f t="shared" si="11"/>
         <v>486.17692072237526</v>
       </c>
-      <c r="AJ13" s="43">
+      <c r="AJ13" s="45" t="e">
+        <f>AC13*1000000/3412/(AA13*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK13" s="43">
         <f t="shared" si="12"/>
-        <v>-133353.3636719824</v>
-      </c>
-      <c r="AK13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL13" t="s">
+        <v>13463.430264501338</v>
+      </c>
+      <c r="AL13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <f t="shared" si="4"/>
         <v>1006.737210423057</v>
       </c>
-      <c r="AN13" s="20">
+      <c r="AO13" s="20">
         <f t="shared" si="13"/>
         <v>10.580318375859296</v>
       </c>
@@ -8004,25 +8056,28 @@
         <f t="shared" si="3"/>
         <v>1296</v>
       </c>
-      <c r="AI14" s="15">
-        <f t="shared" si="11"/>
-        <v>-165.28925619834712</v>
-      </c>
-      <c r="AJ14" s="43">
+      <c r="AI14" s="48">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="45">
+        <f>AC14*1000000/3412/(AA14*3.51)</f>
+        <v>4226.4346554037284</v>
+      </c>
+      <c r="AK14" s="43">
         <f t="shared" si="12"/>
-        <v>-143120.60680523934</v>
-      </c>
-      <c r="AK14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL14" t="s">
+        <v>-135060.69616716646</v>
+      </c>
+      <c r="AL14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <f t="shared" si="4"/>
         <v>1225.8423051598711</v>
       </c>
-      <c r="AN14" s="20">
+      <c r="AO14" s="20">
         <f t="shared" si="13"/>
         <v>11.425171879549596</v>
       </c>
@@ -8138,21 +8193,25 @@
         <f t="shared" si="11"/>
         <v>223.15273951637587</v>
       </c>
-      <c r="AJ15" s="43">
+      <c r="AJ15" s="45">
+        <f>AC15*1000000/3412/(AA15*3.51)</f>
+        <v>32.509435696537871</v>
+      </c>
+      <c r="AK15" s="43">
         <f t="shared" si="12"/>
-        <v>-116051.7962042352</v>
-      </c>
-      <c r="AK15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL15" t="s">
+        <v>13374.910591332446</v>
+      </c>
+      <c r="AL15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM15" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <f t="shared" si="4"/>
         <v>732.00852269989878</v>
       </c>
-      <c r="AN15" s="20">
+      <c r="AO15" s="20">
         <f t="shared" si="13"/>
         <v>9.4965995689416474</v>
       </c>
@@ -8268,26 +8327,30 @@
         <f t="shared" si="11"/>
         <v>429.15824915824919</v>
       </c>
-      <c r="AJ16" s="43">
+      <c r="AJ16" s="45">
+        <f>AC16*1000000/3412/(AA16*3.51)</f>
+        <v>9.4812033082491265</v>
+      </c>
+      <c r="AK16" s="43">
         <f t="shared" si="12"/>
-        <v>-95823.919826679979</v>
-      </c>
-      <c r="AK16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM16">
+        <v>244784.12716568841</v>
+      </c>
+      <c r="AL16" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN16">
         <f t="shared" si="4"/>
         <v>588.85162021330825</v>
       </c>
-      <c r="AN16" s="20">
+      <c r="AO16" s="20">
         <f t="shared" si="13"/>
         <v>8.4990327509480341</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -8401,26 +8464,30 @@
         <f t="shared" si="11"/>
         <v>141.05907560453016</v>
       </c>
-      <c r="AJ17" s="43">
+      <c r="AJ17" s="45">
+        <f>AC17*1000000/3412/(AA17*3.51)</f>
+        <v>5.8809075362836879E-4</v>
+      </c>
+      <c r="AK17" s="43">
         <f t="shared" si="12"/>
-        <v>-80327.097696000012</v>
-      </c>
-      <c r="AK17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM17">
+        <v>20814.567831297958</v>
+      </c>
+      <c r="AL17" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN17">
         <f t="shared" si="4"/>
         <v>3.345699036973989E-2</v>
       </c>
-      <c r="AN17" s="20">
+      <c r="AO17" s="20">
         <f t="shared" si="13"/>
         <v>8.3238659855175783</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -8531,26 +8598,30 @@
         <f t="shared" si="11"/>
         <v>634.02203856749315</v>
       </c>
-      <c r="AJ18" s="43">
+      <c r="AJ18" s="45">
+        <f>AC18*1000000/3412/(AA18*3.51)</f>
+        <v>29.297636439288823</v>
+      </c>
+      <c r="AK18" s="43">
         <f t="shared" si="12"/>
-        <v>-101745.62471191998</v>
-      </c>
-      <c r="AK18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM18">
+        <v>165327.30968332032</v>
+      </c>
+      <c r="AL18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM18" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN18">
         <f t="shared" si="4"/>
         <v>656.68929775282777</v>
       </c>
-      <c r="AN18" s="20">
+      <c r="AO18" s="20">
         <f t="shared" si="13"/>
         <v>11.628845449912982</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -8664,26 +8735,30 @@
         <f t="shared" si="11"/>
         <v>708.68724426288315</v>
       </c>
-      <c r="AJ19" s="43">
+      <c r="AJ19" s="46">
+        <f>AC19*1000000/3412/(AA19*3.51)</f>
+        <v>2.3389661640500456</v>
+      </c>
+      <c r="AK19" s="47">
         <f t="shared" si="12"/>
-        <v>-92225.795841444604</v>
-      </c>
-      <c r="AK19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL19" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM19">
+        <v>54869.326939060469</v>
+      </c>
+      <c r="AL19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN19">
         <f t="shared" si="4"/>
         <v>367.25358157081911</v>
       </c>
-      <c r="AN19" s="20">
+      <c r="AO19" s="20">
         <f t="shared" si="13"/>
         <v>10.637554178269381</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -8800,26 +8875,30 @@
         <f t="shared" si="11"/>
         <v>695.63145903131124</v>
       </c>
-      <c r="AJ20" s="43">
+      <c r="AJ20" s="45" t="e">
+        <f>AC20*1000000/3412/(AA20*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK20" s="43">
         <f t="shared" si="12"/>
-        <v>-90451.180282262489</v>
-      </c>
-      <c r="AK20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM20">
+        <v>-87727.789110590616</v>
+      </c>
+      <c r="AL20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN20">
         <f t="shared" si="4"/>
         <v>954.22971433417922</v>
       </c>
-      <c r="AN20" s="20">
+      <c r="AO20" s="20">
         <f t="shared" si="13"/>
         <v>10.65634629031317</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -8933,26 +9012,30 @@
         <f t="shared" si="11"/>
         <v>371.55800428527704</v>
       </c>
-      <c r="AJ21" s="43">
+      <c r="AJ21" s="45">
+        <f>AC21*1000000/3412/(AA21*3.51)</f>
+        <v>29.476861822620329</v>
+      </c>
+      <c r="AK21" s="43">
         <f t="shared" si="12"/>
-        <v>-74494.838349119993</v>
-      </c>
-      <c r="AK21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL21" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM21">
+        <v>16989.016690890407</v>
+      </c>
+      <c r="AL21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN21">
         <f t="shared" si="4"/>
         <v>390.56047819407189</v>
       </c>
-      <c r="AN21" s="20">
+      <c r="AO21" s="20">
         <f t="shared" si="13"/>
         <v>9.3864719608475653</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -9066,26 +9149,30 @@
         <f t="shared" si="11"/>
         <v>19.151821242730335</v>
       </c>
-      <c r="AJ22" s="43">
+      <c r="AJ22" s="45">
+        <f>AC22*1000000/3412/(AA22*3.51)</f>
+        <v>0.14332700531579684</v>
+      </c>
+      <c r="AK22" s="43">
         <f t="shared" si="12"/>
-        <v>-61409.294724719948</v>
-      </c>
-      <c r="AK22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL22" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM22">
+        <v>10816.715534720846</v>
+      </c>
+      <c r="AL22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM22" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN22">
         <f t="shared" si="4"/>
         <v>3.8135314790130992</v>
       </c>
-      <c r="AN22" s="20">
+      <c r="AO22" s="20">
         <f t="shared" si="13"/>
         <v>8.9124068819447313</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -9196,26 +9283,30 @@
         <f t="shared" si="11"/>
         <v>238.66544230180597</v>
       </c>
-      <c r="AJ23" s="43">
+      <c r="AJ23" s="45">
+        <f>AC23*1000000/3412/(AA23*3.51)</f>
+        <v>16.973292626334992</v>
+      </c>
+      <c r="AK23" s="43">
         <f t="shared" si="12"/>
-        <v>-81916.883393707976</v>
-      </c>
-      <c r="AK23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL23" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM23">
+        <v>-26660.998588201663</v>
+      </c>
+      <c r="AL23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM23" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN23">
         <f t="shared" si="4"/>
         <v>337.41772450978823</v>
       </c>
-      <c r="AN23" s="20">
+      <c r="AO23" s="20">
         <f t="shared" si="13"/>
         <v>14.298596895962708</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -9323,26 +9414,30 @@
         <f t="shared" si="11"/>
         <v>144.0220385674931</v>
       </c>
-      <c r="AJ24" s="43">
+      <c r="AJ24" s="46">
+        <f>AC24*1000000/3412/(AA24*3.51)</f>
+        <v>0.72845373461518059</v>
+      </c>
+      <c r="AK24" s="47">
         <f t="shared" si="12"/>
-        <v>-44288.984129999997</v>
-      </c>
-      <c r="AK24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM24">
+        <v>11721.439713801661</v>
+      </c>
+      <c r="AL24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM24" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN24">
         <f t="shared" si="4"/>
         <v>13.098411729753167</v>
       </c>
-      <c r="AN24" s="20">
+      <c r="AO24" s="20">
         <f t="shared" si="13"/>
         <v>15.95338754168257</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -9398,7 +9493,7 @@
         <v>130</v>
       </c>
       <c r="S25" s="11">
-        <v>100</v>
+        <v>99.9</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>254</v>
@@ -9434,11 +9529,11 @@
       </c>
       <c r="AC25" s="42">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.9724999999997828</v>
       </c>
       <c r="AD25" s="7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.2517123287668753E-4</v>
       </c>
       <c r="AE25" s="42">
         <f t="shared" si="2"/>
@@ -9449,7 +9544,7 @@
       </c>
       <c r="AG25" s="15">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.6195739453013258E-2</v>
       </c>
       <c r="AH25" s="15">
         <f t="shared" si="3"/>
@@ -9459,26 +9554,30 @@
         <f t="shared" si="11"/>
         <v>790.24487297214569</v>
       </c>
-      <c r="AJ25" s="43">
+      <c r="AJ25" s="45">
+        <f>AC25*1000000/3412/(AA25*3.51)</f>
+        <v>1.4645208924187635E-4</v>
+      </c>
+      <c r="AK25" s="43">
         <f t="shared" si="12"/>
-        <v>-192094.58399999997</v>
-      </c>
-      <c r="AK25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL25" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM25">
+        <v>213533.39047983513</v>
+      </c>
+      <c r="AL25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM25" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN25">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN25" s="20">
+        <v>6.5993913504304669E-2</v>
+      </c>
+      <c r="AO25" s="20">
         <f t="shared" si="13"/>
         <v>10.787846258660338</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -9595,26 +9694,30 @@
         <f t="shared" si="11"/>
         <v>625.40404040404042</v>
       </c>
-      <c r="AJ26" s="43">
+      <c r="AJ26" s="45" t="e">
+        <f>AC26*1000000/3412/(AA26*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK26" s="43">
         <f t="shared" si="12"/>
-        <v>-128104.688798912</v>
-      </c>
-      <c r="AK26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL26" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM26">
+        <v>-215866.05293645698</v>
+      </c>
+      <c r="AL26" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM26" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN26">
         <f t="shared" si="4"/>
         <v>1415.0259358589346</v>
       </c>
-      <c r="AN26" s="20">
+      <c r="AO26" s="20">
         <f t="shared" si="13"/>
         <v>8.4036950377424944</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -9731,26 +9834,30 @@
         <f t="shared" si="11"/>
         <v>58.259871441689626</v>
       </c>
-      <c r="AJ27" s="43">
+      <c r="AJ27" s="45" t="e">
+        <f>AC27*1000000/3412/(AA27*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK27" s="43">
         <f t="shared" si="12"/>
-        <v>-28890.618496786999</v>
-      </c>
-      <c r="AK27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL27" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM27">
+        <v>8777.7724614635044</v>
+      </c>
+      <c r="AL27" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM27" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN27">
         <f t="shared" si="4"/>
         <v>123.40948478911389</v>
       </c>
-      <c r="AN27" s="20">
+      <c r="AO27" s="20">
         <f t="shared" si="13"/>
         <v>11.903889474677138</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -9867,38 +9974,42 @@
         <f t="shared" si="11"/>
         <v>182.32224396607961</v>
       </c>
-      <c r="AJ28" s="43">
+      <c r="AJ28" s="45" t="e">
+        <f>AC28*1000000/3412/(AA28*3.51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AK28" s="43">
         <f t="shared" si="12"/>
-        <v>-31164.113877439999</v>
-      </c>
-      <c r="AK28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL28" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM28">
+        <v>-3855.9764027152414</v>
+      </c>
+      <c r="AL28" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM28" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="AN28">
         <f t="shared" si="4"/>
         <v>52.731562521747037</v>
       </c>
-      <c r="AN28" s="20">
+      <c r="AO28" s="20">
         <f t="shared" si="13"/>
         <v>13.956148479427549</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="H29" s="4"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="H30" s="4"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="H31" s="4"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="H32" s="4"/>
     </row>
@@ -25860,27 +25971,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="78ce7efe-c353-4cf8-9d4c-148e26a147e3" xsi:nil="true"/>
-    <Dataextractedfrom50statebiogasprofilesinpdf xmlns="65950468-3135-4891-ae74-8a1589473272" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65950468-3135-4891-ae74-8a1589473272">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EA8C0B3A98985478596F957EEE5A42B" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="813a874e57bc7ee77ed2d675827f2fdd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65950468-3135-4891-ae74-8a1589473272" xmlns:ns3="78ce7efe-c353-4cf8-9d4c-148e26a147e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52589cb147cfc41901144a84263f1621" ns2:_="" ns3:_="">
     <xsd:import namespace="65950468-3135-4891-ae74-8a1589473272"/>
@@ -26107,32 +26197,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE0FBAF-579E-429E-B254-9759185C8EB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="65950468-3135-4891-ae74-8a1589473272"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="78ce7efe-c353-4cf8-9d4c-148e26a147e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D085DC7-2B76-4A87-9F5C-038FAA97CFCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="78ce7efe-c353-4cf8-9d4c-148e26a147e3" xsi:nil="true"/>
+    <Dataextractedfrom50statebiogasprofilesinpdf xmlns="65950468-3135-4891-ae74-8a1589473272" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65950468-3135-4891-ae74-8a1589473272">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47952F0A-656C-49A9-873F-B128AEF0E2E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26149,4 +26235,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D085DC7-2B76-4A87-9F5C-038FAA97CFCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AE0FBAF-579E-429E-B254-9759185C8EB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="65950468-3135-4891-ae74-8a1589473272"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="78ce7efe-c353-4cf8-9d4c-148e26a147e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>